<commit_message>
Compilation of cubist model as provided by Bo Andree
</commit_message>
<xml_diff>
--- a/data/Calibration/Calibration_continents_20250901.xlsx
+++ b/data/Calibration/Calibration_continents_20250901.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projdir\2burp\Data\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{995E16A8-F547-4444-BF11-D1FEE7E93EEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3AE523-E083-48F8-8BC9-197FFD745B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="autoglm" sheetId="9" r:id="rId1"/>
     <sheet name="glm2" sheetId="10" r:id="rId2"/>
+    <sheet name="beta" sheetId="12" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>ln_PopulationDensity_2000_8dir</t>
   </si>
@@ -110,7 +111,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.00000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,6 +123,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -147,7 +155,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -166,6 +174,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -847,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C56D62-ACCE-4699-9A74-008731C7F163}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1229,4 +1239,394 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2288A177-213B-40FC-8365-96A4EFE9B64C}">
+  <dimension ref="A1:G17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8">
+        <v>-1.6611291349999999</v>
+      </c>
+      <c r="C2" s="8">
+        <v>-1.6611291349999999</v>
+      </c>
+      <c r="D2" s="8">
+        <v>-1.6611291349999999</v>
+      </c>
+      <c r="E2" s="8">
+        <v>-1.6611291349999999</v>
+      </c>
+      <c r="F2" s="8">
+        <v>-1.6611291349999999</v>
+      </c>
+      <c r="G2" s="8">
+        <v>-1.6611291349999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="8">
+        <v>5.344501631</v>
+      </c>
+      <c r="C3" s="8">
+        <v>5.344501631</v>
+      </c>
+      <c r="D3" s="8">
+        <v>5.344501631</v>
+      </c>
+      <c r="E3" s="8">
+        <v>5.344501631</v>
+      </c>
+      <c r="F3" s="8">
+        <v>5.344501631</v>
+      </c>
+      <c r="G3" s="8">
+        <v>5.344501631</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="8">
+        <v>4.3162310000000002E-2</v>
+      </c>
+      <c r="C4" s="8">
+        <v>4.3162310000000002E-2</v>
+      </c>
+      <c r="D4" s="8">
+        <v>4.3162310000000002E-2</v>
+      </c>
+      <c r="E4" s="8">
+        <v>4.3162310000000002E-2</v>
+      </c>
+      <c r="F4" s="8">
+        <v>4.3162310000000002E-2</v>
+      </c>
+      <c r="G4" s="8">
+        <v>4.3162310000000002E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="9">
+        <v>8.4400000000000005E-5</v>
+      </c>
+      <c r="C5" s="9">
+        <v>8.4400000000000005E-5</v>
+      </c>
+      <c r="D5" s="9">
+        <v>8.4400000000000005E-5</v>
+      </c>
+      <c r="E5" s="9">
+        <v>8.4400000000000005E-5</v>
+      </c>
+      <c r="F5" s="9">
+        <v>8.4400000000000005E-5</v>
+      </c>
+      <c r="G5" s="9">
+        <v>8.4400000000000005E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9">
+        <v>-8.9599999999999996E-5</v>
+      </c>
+      <c r="C6" s="9">
+        <v>-8.9599999999999996E-5</v>
+      </c>
+      <c r="D6" s="9">
+        <v>-8.9599999999999996E-5</v>
+      </c>
+      <c r="E6" s="9">
+        <v>-8.9599999999999996E-5</v>
+      </c>
+      <c r="F6" s="9">
+        <v>-8.9599999999999996E-5</v>
+      </c>
+      <c r="G6" s="9">
+        <v>-8.9599999999999996E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="8">
+        <v>-1.5118600000000001E-4</v>
+      </c>
+      <c r="C7" s="8">
+        <v>-1.5118600000000001E-4</v>
+      </c>
+      <c r="D7" s="8">
+        <v>-1.5118600000000001E-4</v>
+      </c>
+      <c r="E7" s="8">
+        <v>-1.5118600000000001E-4</v>
+      </c>
+      <c r="F7" s="8">
+        <v>-1.5118600000000001E-4</v>
+      </c>
+      <c r="G7" s="8">
+        <v>-1.5118600000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="8">
+        <v>-2.62212E-4</v>
+      </c>
+      <c r="C8" s="8">
+        <v>-2.62212E-4</v>
+      </c>
+      <c r="D8" s="8">
+        <v>-2.62212E-4</v>
+      </c>
+      <c r="E8" s="8">
+        <v>-2.62212E-4</v>
+      </c>
+      <c r="F8" s="8">
+        <v>-2.62212E-4</v>
+      </c>
+      <c r="G8" s="8">
+        <v>-2.62212E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="8">
+        <v>-2.6221399999999998E-4</v>
+      </c>
+      <c r="C9" s="8">
+        <v>-2.6221399999999998E-4</v>
+      </c>
+      <c r="D9" s="8">
+        <v>-2.6221399999999998E-4</v>
+      </c>
+      <c r="E9" s="8">
+        <v>-2.6221399999999998E-4</v>
+      </c>
+      <c r="F9" s="8">
+        <v>-2.6221399999999998E-4</v>
+      </c>
+      <c r="G9" s="8">
+        <v>-2.6221399999999998E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="9">
+        <v>3.1199999999999999E-7</v>
+      </c>
+      <c r="C10" s="9">
+        <v>3.1199999999999999E-7</v>
+      </c>
+      <c r="D10" s="9">
+        <v>3.1199999999999999E-7</v>
+      </c>
+      <c r="E10" s="9">
+        <v>3.1199999999999999E-7</v>
+      </c>
+      <c r="F10" s="9">
+        <v>3.1199999999999999E-7</v>
+      </c>
+      <c r="G10" s="9">
+        <v>3.1199999999999999E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="8">
+        <v>-1.4168080000000001E-3</v>
+      </c>
+      <c r="C11" s="8">
+        <v>-1.4168080000000001E-3</v>
+      </c>
+      <c r="D11" s="8">
+        <v>-1.4168080000000001E-3</v>
+      </c>
+      <c r="E11" s="8">
+        <v>-1.4168080000000001E-3</v>
+      </c>
+      <c r="F11" s="8">
+        <v>-1.4168080000000001E-3</v>
+      </c>
+      <c r="G11" s="8">
+        <v>-1.4168080000000001E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="8">
+        <v>-3.5518428999999997E-2</v>
+      </c>
+      <c r="C12" s="8">
+        <v>-3.5518428999999997E-2</v>
+      </c>
+      <c r="D12" s="8">
+        <v>-3.5518428999999997E-2</v>
+      </c>
+      <c r="E12" s="8">
+        <v>-3.5518428999999997E-2</v>
+      </c>
+      <c r="F12" s="8">
+        <v>-3.5518428999999997E-2</v>
+      </c>
+      <c r="G12" s="8">
+        <v>-3.5518428999999997E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="8">
+        <v>-1.5794656000000001E-2</v>
+      </c>
+      <c r="C13" s="8">
+        <v>-1.5794656000000001E-2</v>
+      </c>
+      <c r="D13" s="8">
+        <v>-1.5794656000000001E-2</v>
+      </c>
+      <c r="E13" s="8">
+        <v>-1.5794656000000001E-2</v>
+      </c>
+      <c r="F13" s="8">
+        <v>-1.5794656000000001E-2</v>
+      </c>
+      <c r="G13" s="8">
+        <v>-1.5794656000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="8">
+        <v>-1.1395384E-2</v>
+      </c>
+      <c r="C14" s="8">
+        <v>-1.1395384E-2</v>
+      </c>
+      <c r="D14" s="8">
+        <v>-1.1395384E-2</v>
+      </c>
+      <c r="E14" s="8">
+        <v>-1.1395384E-2</v>
+      </c>
+      <c r="F14" s="8">
+        <v>-1.1395384E-2</v>
+      </c>
+      <c r="G14" s="8">
+        <v>-1.1395384E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" s="8">
+        <v>-4.0323520000000003E-3</v>
+      </c>
+      <c r="C15" s="8">
+        <v>-4.0323520000000003E-3</v>
+      </c>
+      <c r="D15" s="8">
+        <v>-4.0323520000000003E-3</v>
+      </c>
+      <c r="E15" s="8">
+        <v>-4.0323520000000003E-3</v>
+      </c>
+      <c r="F15" s="8">
+        <v>-4.0323520000000003E-3</v>
+      </c>
+      <c r="G15" s="8">
+        <v>-4.0323520000000003E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="8">
+        <v>-5.1937540000000001E-3</v>
+      </c>
+      <c r="C16" s="8">
+        <v>-5.1937540000000001E-3</v>
+      </c>
+      <c r="D16" s="8">
+        <v>-5.1937540000000001E-3</v>
+      </c>
+      <c r="E16" s="8">
+        <v>-5.1937540000000001E-3</v>
+      </c>
+      <c r="F16" s="8">
+        <v>-5.1937540000000001E-3</v>
+      </c>
+      <c r="G16" s="8">
+        <v>-5.1937540000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated beta and glm models (both with logit link now)
</commit_message>
<xml_diff>
--- a/data/Calibration/Calibration_continents_20250901.xlsx
+++ b/data/Calibration/Calibration_continents_20250901.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\projdir\2burp\Data\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA3AE523-E083-48F8-8BC9-197FFD745B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0067E68-4DE8-4D4F-B5F8-0D14A31FE8EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="autoglm" sheetId="9" r:id="rId1"/>
@@ -857,8 +857,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76C56D62-ACCE-4699-9A74-008731C7F163}">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:G1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,8 +895,8 @@
       <c r="A2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="B2">
-        <v>-2.6562552545607399</v>
+      <c r="B2" s="8">
+        <v>-5.3013505529999998</v>
       </c>
       <c r="C2">
         <v>-2.6562552545607399</v>
@@ -918,8 +918,8 @@
       <c r="A3" t="s">
         <v>24</v>
       </c>
-      <c r="B3">
-        <v>4.6021488337660204</v>
+      <c r="B3" s="8">
+        <v>7.2650027279999998</v>
       </c>
       <c r="C3">
         <v>4.6021488337660204</v>
@@ -941,8 +941,8 @@
       <c r="A4" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
-        <v>0.16734036683046999</v>
+      <c r="B4" s="8">
+        <v>0.44098974499999999</v>
       </c>
       <c r="C4">
         <v>0.16734036683046999</v>
@@ -964,8 +964,8 @@
       <c r="A5" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6">
-        <v>6.7761525883721298E-5</v>
+      <c r="B5" s="8">
+        <v>2.3276699999999999E-4</v>
       </c>
       <c r="C5" s="6">
         <v>6.7761525883721298E-5</v>
@@ -987,8 +987,8 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
-        <v>-2.4667285489229798E-4</v>
+      <c r="B6" s="8">
+        <v>-6.7812999999999999E-4</v>
       </c>
       <c r="C6">
         <v>-2.4667285489229798E-4</v>
@@ -1010,8 +1010,8 @@
       <c r="A7" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
-        <v>-9.4190995355361096E-4</v>
+      <c r="B7" s="8">
+        <v>-3.050189E-3</v>
       </c>
       <c r="C7">
         <v>-9.4190995355361096E-4</v>
@@ -1033,8 +1033,8 @@
       <c r="A8" t="s">
         <v>21</v>
       </c>
-      <c r="B8">
-        <v>1.1289487945175E-4</v>
+      <c r="B8" s="8">
+        <v>1.177158E-3</v>
       </c>
       <c r="C8">
         <v>1.1289487945175E-4</v>
@@ -1056,8 +1056,8 @@
       <c r="A9" t="s">
         <v>22</v>
       </c>
-      <c r="B9">
-        <v>-3.5444331299824398E-3</v>
+      <c r="B9" s="8">
+        <v>-1.3657028E-2</v>
       </c>
       <c r="C9">
         <v>-3.5444331299824398E-3</v>
@@ -1079,8 +1079,8 @@
       <c r="A10" t="s">
         <v>3</v>
       </c>
-      <c r="B10" s="6">
-        <v>2.41760990893255E-5</v>
+      <c r="B10" s="9">
+        <v>3.2400000000000001E-5</v>
       </c>
       <c r="C10" s="6">
         <v>2.41760990893255E-5</v>
@@ -1102,8 +1102,8 @@
       <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B11">
-        <v>-1.06067228686963E-2</v>
+      <c r="B11" s="8">
+        <v>-2.5872468999999999E-2</v>
       </c>
       <c r="C11">
         <v>-1.06067228686963E-2</v>
@@ -1125,8 +1125,8 @@
       <c r="A12" t="s">
         <v>12</v>
       </c>
-      <c r="B12">
-        <v>-0.2076612979944</v>
+      <c r="B12" s="8">
+        <v>-0.62798805800000002</v>
       </c>
       <c r="C12">
         <v>-0.2076612979944</v>
@@ -1148,8 +1148,8 @@
       <c r="A13" t="s">
         <v>4</v>
       </c>
-      <c r="B13">
-        <v>-7.5823839215900302E-2</v>
+      <c r="B13" s="8">
+        <v>-0.18155501499999999</v>
       </c>
       <c r="C13">
         <v>-7.5823839215900302E-2</v>
@@ -1171,8 +1171,8 @@
       <c r="A14" t="s">
         <v>5</v>
       </c>
-      <c r="B14">
-        <v>-1.52790331966727E-2</v>
+      <c r="B14" s="8">
+        <v>-3.6474089000000001E-2</v>
       </c>
       <c r="C14">
         <v>-1.52790331966727E-2</v>
@@ -1194,8 +1194,8 @@
       <c r="A15" t="s">
         <v>6</v>
       </c>
-      <c r="B15">
-        <v>-8.4509741356945008E-3</v>
+      <c r="B15" s="8">
+        <v>-2.1084724999999999E-2</v>
       </c>
       <c r="C15">
         <v>-8.4509741356945008E-3</v>
@@ -1217,8 +1217,8 @@
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16">
-        <v>-4.1242031894640303E-3</v>
+      <c r="B16" s="8">
+        <v>-2.1317490000000001E-3</v>
       </c>
       <c r="C16">
         <v>-4.1242031894640303E-3</v>
@@ -1243,10 +1243,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2288A177-213B-40FC-8365-96A4EFE9B64C}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:G16"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:XFD46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1282,22 +1282,22 @@
         <v>19</v>
       </c>
       <c r="B2" s="8">
-        <v>-1.6611291349999999</v>
+        <v>-5.0331725220000001</v>
       </c>
       <c r="C2" s="8">
-        <v>-1.6611291349999999</v>
+        <v>-5.3013505529999998</v>
       </c>
       <c r="D2" s="8">
-        <v>-1.6611291349999999</v>
+        <v>-5.3013505529999998</v>
       </c>
       <c r="E2" s="8">
-        <v>-1.6611291349999999</v>
+        <v>-5.3013505529999998</v>
       </c>
       <c r="F2" s="8">
-        <v>-1.6611291349999999</v>
+        <v>-5.3013505529999998</v>
       </c>
       <c r="G2" s="8">
-        <v>-1.6611291349999999</v>
+        <v>-5.3013505529999998</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1305,22 +1305,22 @@
         <v>24</v>
       </c>
       <c r="B3" s="8">
-        <v>5.344501631</v>
+        <v>9.9790316990000001</v>
       </c>
       <c r="C3" s="8">
-        <v>5.344501631</v>
+        <v>7.2650027279999998</v>
       </c>
       <c r="D3" s="8">
-        <v>5.344501631</v>
+        <v>7.2650027279999998</v>
       </c>
       <c r="E3" s="8">
-        <v>5.344501631</v>
+        <v>7.2650027279999998</v>
       </c>
       <c r="F3" s="8">
-        <v>5.344501631</v>
+        <v>7.2650027279999998</v>
       </c>
       <c r="G3" s="8">
-        <v>5.344501631</v>
+        <v>7.2650027279999998</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1328,68 +1328,68 @@
         <v>0</v>
       </c>
       <c r="B4" s="8">
-        <v>4.3162310000000002E-2</v>
+        <v>0.26250815</v>
       </c>
       <c r="C4" s="8">
-        <v>4.3162310000000002E-2</v>
+        <v>0.44098974499999999</v>
       </c>
       <c r="D4" s="8">
-        <v>4.3162310000000002E-2</v>
+        <v>0.44098974499999999</v>
       </c>
       <c r="E4" s="8">
-        <v>4.3162310000000002E-2</v>
+        <v>0.44098974499999999</v>
       </c>
       <c r="F4" s="8">
-        <v>4.3162310000000002E-2</v>
+        <v>0.44098974499999999</v>
       </c>
       <c r="G4" s="8">
-        <v>4.3162310000000002E-2</v>
+        <v>0.44098974499999999</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="9">
-        <v>8.4400000000000005E-5</v>
-      </c>
-      <c r="C5" s="9">
-        <v>8.4400000000000005E-5</v>
-      </c>
-      <c r="D5" s="9">
-        <v>8.4400000000000005E-5</v>
-      </c>
-      <c r="E5" s="9">
-        <v>8.4400000000000005E-5</v>
-      </c>
-      <c r="F5" s="9">
-        <v>8.4400000000000005E-5</v>
-      </c>
-      <c r="G5" s="9">
-        <v>8.4400000000000005E-5</v>
+      <c r="B5" s="8">
+        <v>3.6590700000000001E-4</v>
+      </c>
+      <c r="C5" s="8">
+        <v>2.3276699999999999E-4</v>
+      </c>
+      <c r="D5" s="8">
+        <v>2.3276699999999999E-4</v>
+      </c>
+      <c r="E5" s="8">
+        <v>2.3276699999999999E-4</v>
+      </c>
+      <c r="F5" s="8">
+        <v>2.3276699999999999E-4</v>
+      </c>
+      <c r="G5" s="8">
+        <v>2.3276699999999999E-4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="9">
-        <v>-8.9599999999999996E-5</v>
-      </c>
-      <c r="C6" s="9">
-        <v>-8.9599999999999996E-5</v>
-      </c>
-      <c r="D6" s="9">
-        <v>-8.9599999999999996E-5</v>
-      </c>
-      <c r="E6" s="9">
-        <v>-8.9599999999999996E-5</v>
-      </c>
-      <c r="F6" s="9">
-        <v>-8.9599999999999996E-5</v>
-      </c>
-      <c r="G6" s="9">
-        <v>-8.9599999999999996E-5</v>
+      <c r="B6" s="8">
+        <v>-6.5139199999999999E-4</v>
+      </c>
+      <c r="C6" s="8">
+        <v>-6.7812999999999999E-4</v>
+      </c>
+      <c r="D6" s="8">
+        <v>-6.7812999999999999E-4</v>
+      </c>
+      <c r="E6" s="8">
+        <v>-6.7812999999999999E-4</v>
+      </c>
+      <c r="F6" s="8">
+        <v>-6.7812999999999999E-4</v>
+      </c>
+      <c r="G6" s="8">
+        <v>-6.7812999999999999E-4</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1397,22 +1397,22 @@
         <v>11</v>
       </c>
       <c r="B7" s="8">
-        <v>-1.5118600000000001E-4</v>
+        <v>-8.4075100000000004E-4</v>
       </c>
       <c r="C7" s="8">
-        <v>-1.5118600000000001E-4</v>
+        <v>-3.050189E-3</v>
       </c>
       <c r="D7" s="8">
-        <v>-1.5118600000000001E-4</v>
+        <v>-3.050189E-3</v>
       </c>
       <c r="E7" s="8">
-        <v>-1.5118600000000001E-4</v>
+        <v>-3.050189E-3</v>
       </c>
       <c r="F7" s="8">
-        <v>-1.5118600000000001E-4</v>
+        <v>-3.050189E-3</v>
       </c>
       <c r="G7" s="8">
-        <v>-1.5118600000000001E-4</v>
+        <v>-3.050189E-3</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -1420,22 +1420,22 @@
         <v>21</v>
       </c>
       <c r="B8" s="8">
-        <v>-2.62212E-4</v>
+        <v>-3.2050699999999999E-4</v>
       </c>
       <c r="C8" s="8">
-        <v>-2.62212E-4</v>
+        <v>1.177158E-3</v>
       </c>
       <c r="D8" s="8">
-        <v>-2.62212E-4</v>
+        <v>1.177158E-3</v>
       </c>
       <c r="E8" s="8">
-        <v>-2.62212E-4</v>
+        <v>1.177158E-3</v>
       </c>
       <c r="F8" s="8">
-        <v>-2.62212E-4</v>
+        <v>1.177158E-3</v>
       </c>
       <c r="G8" s="8">
-        <v>-2.62212E-4</v>
+        <v>1.177158E-3</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1443,22 +1443,22 @@
         <v>22</v>
       </c>
       <c r="B9" s="8">
-        <v>-2.6221399999999998E-4</v>
+        <v>-2.2758539999999999E-3</v>
       </c>
       <c r="C9" s="8">
-        <v>-2.6221399999999998E-4</v>
+        <v>-1.3657028E-2</v>
       </c>
       <c r="D9" s="8">
-        <v>-2.6221399999999998E-4</v>
+        <v>-1.3657028E-2</v>
       </c>
       <c r="E9" s="8">
-        <v>-2.6221399999999998E-4</v>
+        <v>-1.3657028E-2</v>
       </c>
       <c r="F9" s="8">
-        <v>-2.6221399999999998E-4</v>
+        <v>-1.3657028E-2</v>
       </c>
       <c r="G9" s="8">
-        <v>-2.6221399999999998E-4</v>
+        <v>-1.3657028E-2</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1466,22 +1466,22 @@
         <v>3</v>
       </c>
       <c r="B10" s="9">
-        <v>3.1199999999999999E-7</v>
+        <v>6.3600000000000001E-6</v>
       </c>
       <c r="C10" s="9">
-        <v>3.1199999999999999E-7</v>
+        <v>3.2400000000000001E-5</v>
       </c>
       <c r="D10" s="9">
-        <v>3.1199999999999999E-7</v>
+        <v>3.2400000000000001E-5</v>
       </c>
       <c r="E10" s="9">
-        <v>3.1199999999999999E-7</v>
+        <v>3.2400000000000001E-5</v>
       </c>
       <c r="F10" s="9">
-        <v>3.1199999999999999E-7</v>
+        <v>3.2400000000000001E-5</v>
       </c>
       <c r="G10" s="9">
-        <v>3.1199999999999999E-7</v>
+        <v>3.2400000000000001E-5</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1489,22 +1489,22 @@
         <v>17</v>
       </c>
       <c r="B11" s="8">
-        <v>-1.4168080000000001E-3</v>
+        <v>-1.4953315999999999E-2</v>
       </c>
       <c r="C11" s="8">
-        <v>-1.4168080000000001E-3</v>
+        <v>-2.5872468999999999E-2</v>
       </c>
       <c r="D11" s="8">
-        <v>-1.4168080000000001E-3</v>
+        <v>-2.5872468999999999E-2</v>
       </c>
       <c r="E11" s="8">
-        <v>-1.4168080000000001E-3</v>
+        <v>-2.5872468999999999E-2</v>
       </c>
       <c r="F11" s="8">
-        <v>-1.4168080000000001E-3</v>
+        <v>-2.5872468999999999E-2</v>
       </c>
       <c r="G11" s="8">
-        <v>-1.4168080000000001E-3</v>
+        <v>-2.5872468999999999E-2</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1512,22 +1512,22 @@
         <v>12</v>
       </c>
       <c r="B12" s="8">
-        <v>-3.5518428999999997E-2</v>
+        <v>-0.250141893</v>
       </c>
       <c r="C12" s="8">
-        <v>-3.5518428999999997E-2</v>
+        <v>-0.62798805800000002</v>
       </c>
       <c r="D12" s="8">
-        <v>-3.5518428999999997E-2</v>
+        <v>-0.62798805800000002</v>
       </c>
       <c r="E12" s="8">
-        <v>-3.5518428999999997E-2</v>
+        <v>-0.62798805800000002</v>
       </c>
       <c r="F12" s="8">
-        <v>-3.5518428999999997E-2</v>
+        <v>-0.62798805800000002</v>
       </c>
       <c r="G12" s="8">
-        <v>-3.5518428999999997E-2</v>
+        <v>-0.62798805800000002</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1535,22 +1535,22 @@
         <v>4</v>
       </c>
       <c r="B13" s="8">
-        <v>-1.5794656000000001E-2</v>
+        <v>-0.10437049700000001</v>
       </c>
       <c r="C13" s="8">
-        <v>-1.5794656000000001E-2</v>
+        <v>-0.18155501499999999</v>
       </c>
       <c r="D13" s="8">
-        <v>-1.5794656000000001E-2</v>
+        <v>-0.18155501499999999</v>
       </c>
       <c r="E13" s="8">
-        <v>-1.5794656000000001E-2</v>
+        <v>-0.18155501499999999</v>
       </c>
       <c r="F13" s="8">
-        <v>-1.5794656000000001E-2</v>
+        <v>-0.18155501499999999</v>
       </c>
       <c r="G13" s="8">
-        <v>-1.5794656000000001E-2</v>
+        <v>-0.18155501499999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1558,22 +1558,22 @@
         <v>5</v>
       </c>
       <c r="B14" s="8">
-        <v>-1.1395384E-2</v>
+        <v>-4.7374274000000001E-2</v>
       </c>
       <c r="C14" s="8">
-        <v>-1.1395384E-2</v>
+        <v>-3.6474089000000001E-2</v>
       </c>
       <c r="D14" s="8">
-        <v>-1.1395384E-2</v>
+        <v>-3.6474089000000001E-2</v>
       </c>
       <c r="E14" s="8">
-        <v>-1.1395384E-2</v>
+        <v>-3.6474089000000001E-2</v>
       </c>
       <c r="F14" s="8">
-        <v>-1.1395384E-2</v>
+        <v>-3.6474089000000001E-2</v>
       </c>
       <c r="G14" s="8">
-        <v>-1.1395384E-2</v>
+        <v>-3.6474089000000001E-2</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1581,22 +1581,22 @@
         <v>6</v>
       </c>
       <c r="B15" s="8">
-        <v>-4.0323520000000003E-3</v>
+        <v>-2.5258572999999999E-2</v>
       </c>
       <c r="C15" s="8">
-        <v>-4.0323520000000003E-3</v>
+        <v>-2.1084724999999999E-2</v>
       </c>
       <c r="D15" s="8">
-        <v>-4.0323520000000003E-3</v>
+        <v>-2.1084724999999999E-2</v>
       </c>
       <c r="E15" s="8">
-        <v>-4.0323520000000003E-3</v>
+        <v>-2.1084724999999999E-2</v>
       </c>
       <c r="F15" s="8">
-        <v>-4.0323520000000003E-3</v>
+        <v>-2.1084724999999999E-2</v>
       </c>
       <c r="G15" s="8">
-        <v>-4.0323520000000003E-3</v>
+        <v>-2.1084724999999999E-2</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1604,27 +1604,23 @@
         <v>23</v>
       </c>
       <c r="B16" s="8">
-        <v>-5.1937540000000001E-3</v>
+        <v>-2.4602938000000001E-2</v>
       </c>
       <c r="C16" s="8">
-        <v>-5.1937540000000001E-3</v>
+        <v>-2.1317490000000001E-3</v>
       </c>
       <c r="D16" s="8">
-        <v>-5.1937540000000001E-3</v>
+        <v>-2.1317490000000001E-3</v>
       </c>
       <c r="E16" s="8">
-        <v>-5.1937540000000001E-3</v>
+        <v>-2.1317490000000001E-3</v>
       </c>
       <c r="F16" s="8">
-        <v>-5.1937540000000001E-3</v>
+        <v>-2.1317490000000001E-3</v>
       </c>
       <c r="G16" s="8">
-        <v>-5.1937540000000001E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="8"/>
+        <v>-2.1317490000000001E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>